<commit_message>
Code updates for Simple shapes project1
</commit_message>
<xml_diff>
--- a/MySEProject/Documentation/Dataset Report/Experiment Report.xlsx
+++ b/MySEProject/Documentation/Dataset Report/Experiment Report.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="165">
   <si>
     <t>Experiment Number</t>
   </si>
@@ -46,18 +46,6 @@
   </si>
   <si>
     <t>32x32</t>
-  </si>
-  <si>
-    <t>output-02</t>
-  </si>
-  <si>
-    <t>output-03</t>
-  </si>
-  <si>
-    <t>output-04</t>
-  </si>
-  <si>
-    <t>output-05</t>
   </si>
   <si>
     <t>circle-rectangle macro correlation is high
@@ -99,39 +87,6 @@
 macro corelation(36-1.8%) micro corelation(81-40%)</t>
   </si>
   <si>
-    <t>output-22</t>
-  </si>
-  <si>
-    <t>output-23</t>
-  </si>
-  <si>
-    <t>output-24</t>
-  </si>
-  <si>
-    <t>output-25</t>
-  </si>
-  <si>
-    <t>output-26</t>
-  </si>
-  <si>
-    <t>output-27</t>
-  </si>
-  <si>
-    <t>output-28</t>
-  </si>
-  <si>
-    <t>output-29</t>
-  </si>
-  <si>
-    <t>output-31</t>
-  </si>
-  <si>
-    <t>output-30</t>
-  </si>
-  <si>
-    <t>output-33</t>
-  </si>
-  <si>
     <t>Both macro and micro corelation are low and almost equal</t>
   </si>
   <si>
@@ -158,17 +113,11 @@
 macro corelation(54-0%) micro corelation(94-63%)</t>
   </si>
   <si>
-    <t>output-34</t>
-  </si>
-  <si>
     <t>valid output, circle-rectangle macro correlation is high
 macro corelation(57-5%) micro corelation(94-61%)</t>
   </si>
   <si>
     <t>Result(micro and macro corelation where the percentages refer to the maximun and minimum values from all the shapes)</t>
-  </si>
-  <si>
-    <t>output-35</t>
   </si>
   <si>
     <t>circle-rectangle macro correlation is high
@@ -354,9 +303,6 @@
     <t>valid output micro(92-75) and macro(68-45)</t>
   </si>
   <si>
-    <t>output01</t>
-  </si>
-  <si>
     <t>output</t>
   </si>
   <si>
@@ -628,6 +574,15 @@
   </si>
   <si>
     <t>output100</t>
+  </si>
+  <si>
+    <t>output22</t>
+  </si>
+  <si>
+    <t>output23</t>
+  </si>
+  <si>
+    <t>output24</t>
   </si>
 </sst>
 </file>
@@ -1075,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N84" sqref="N84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,10 +1059,10 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
       <c r="H1" s="14" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1125,17 +1080,17 @@
         <v>2</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1161,10 +1116,10 @@
         <v>5</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>88</v>
+        <v>162</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1190,10 +1145,10 @@
         <v>5</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>7</v>
+        <v>163</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1218,11 +1173,9 @@
       <c r="G6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1247,11 +1200,9 @@
       <c r="G7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1276,11 +1227,9 @@
       <c r="G8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1288,7 +1237,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="2">
         <v>30</v>
@@ -1306,10 +1255,10 @@
         <v>5</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>21</v>
+        <v>164</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1317,7 +1266,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2">
         <v>30</v>
@@ -1334,11 +1283,9 @@
       <c r="G10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1346,7 +1293,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="2">
         <v>30</v>
@@ -1363,11 +1310,9 @@
       <c r="G11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1375,7 +1320,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="2">
         <v>30</v>
@@ -1387,16 +1332,14 @@
         <v>-1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1404,7 +1347,7 @@
         <v>26</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="2">
         <v>30</v>
@@ -1416,16 +1359,14 @@
         <v>-1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="H13" s="2"/>
       <c r="I13" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1442,16 +1383,14 @@
         <v>-1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1468,16 +1407,14 @@
         <v>-1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1485,7 +1422,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2">
         <v>30</v>
@@ -1494,16 +1431,14 @@
         <v>-1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="H16" s="2"/>
       <c r="I16" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1511,7 +1446,7 @@
         <v>30</v>
       </c>
       <c r="B17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2">
         <v>30</v>
@@ -1520,16 +1455,14 @@
         <v>-1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="H17" s="2"/>
       <c r="I17" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1537,7 +1470,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2">
         <v>30</v>
@@ -1546,16 +1479,14 @@
         <v>-1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="H18" s="2"/>
       <c r="I18" s="2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1563,7 +1494,7 @@
         <v>33</v>
       </c>
       <c r="B19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2">
         <v>30</v>
@@ -1577,11 +1508,9 @@
       <c r="G19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="H19" s="2"/>
       <c r="I19" s="2" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1589,7 +1518,7 @@
         <v>34</v>
       </c>
       <c r="B20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2">
         <v>30</v>
@@ -1603,11 +1532,9 @@
       <c r="G20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="H20" s="2"/>
       <c r="I20" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1615,7 +1542,7 @@
         <v>35</v>
       </c>
       <c r="B21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2">
         <v>30</v>
@@ -1629,16 +1556,14 @@
       <c r="G21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="H21" s="2"/>
       <c r="I21" s="1" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1661,10 +1586,10 @@
         <v>5</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1687,10 +1612,10 @@
         <v>5</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1713,10 +1638,10 @@
         <v>5</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1739,10 +1664,10 @@
         <v>5</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1765,10 +1690,10 @@
         <v>5</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1791,10 +1716,10 @@
         <v>5</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1817,10 +1742,10 @@
         <v>5</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1843,10 +1768,10 @@
         <v>5</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1869,10 +1794,10 @@
         <v>5</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1895,10 +1820,10 @@
         <v>5</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1921,10 +1846,10 @@
         <v>5</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1947,10 +1872,10 @@
         <v>5</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1973,10 +1898,10 @@
         <v>5</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1999,10 +1924,10 @@
         <v>5</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2025,10 +1950,10 @@
         <v>5</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2051,10 +1976,10 @@
         <v>5</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2077,10 +2002,10 @@
         <v>5</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2103,10 +2028,10 @@
         <v>5</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2129,10 +2054,10 @@
         <v>5</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2155,10 +2080,10 @@
         <v>5</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2181,10 +2106,10 @@
         <v>5</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2207,10 +2132,10 @@
         <v>5</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2233,15 +2158,15 @@
         <v>5</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
@@ -2275,10 +2200,10 @@
         <v>5</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2304,10 +2229,10 @@
         <v>5</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2333,10 +2258,10 @@
         <v>5</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2362,10 +2287,10 @@
         <v>5</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2391,10 +2316,10 @@
         <v>5</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2420,10 +2345,10 @@
         <v>5</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2449,10 +2374,10 @@
         <v>5</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2478,10 +2403,10 @@
         <v>5</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2507,10 +2432,10 @@
         <v>5</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2536,10 +2461,10 @@
         <v>5</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2565,10 +2490,10 @@
         <v>5</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2594,10 +2519,10 @@
         <v>5</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2623,10 +2548,10 @@
         <v>5</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2652,10 +2577,10 @@
         <v>5</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2681,10 +2606,10 @@
         <v>5</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2710,10 +2635,10 @@
         <v>5</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2739,10 +2664,10 @@
         <v>5</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2768,10 +2693,10 @@
         <v>5</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2797,10 +2722,10 @@
         <v>5</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2826,10 +2751,10 @@
         <v>5</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2855,10 +2780,10 @@
         <v>5</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2866,44 +2791,16 @@
       <c r="I68" s="2"/>
     </row>
     <row r="69" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
-        <v>14</v>
-      </c>
-      <c r="E69" s="6">
-        <v>-1</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="H69" s="2"/>
-      <c r="I69" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I69" s="2"/>
     </row>
     <row r="70" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
-        <v>15</v>
-      </c>
-      <c r="E70" s="6">
-        <v>-1</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="H70" s="2"/>
-      <c r="I70" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="I70" s="2"/>
     </row>
     <row r="71" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2929,10 +2826,10 @@
         <v>5</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2958,10 +2855,10 @@
         <v>5</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2987,10 +2884,10 @@
         <v>5</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3016,10 +2913,10 @@
         <v>5</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3045,10 +2942,10 @@
         <v>5</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3074,10 +2971,10 @@
         <v>5</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3103,10 +3000,10 @@
         <v>5</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3132,10 +3029,10 @@
         <v>5</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3161,10 +3058,10 @@
         <v>5</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3190,10 +3087,10 @@
         <v>5</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3219,10 +3116,10 @@
         <v>5</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3248,10 +3145,10 @@
         <v>5</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3277,10 +3174,10 @@
         <v>5</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3306,10 +3203,10 @@
         <v>5</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3335,10 +3232,10 @@
         <v>5</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3364,10 +3261,10 @@
         <v>5</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3393,10 +3290,10 @@
         <v>5</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3422,10 +3319,10 @@
         <v>5</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3451,10 +3348,10 @@
         <v>5</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3480,10 +3377,10 @@
         <v>5</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3496,7 +3393,7 @@
     </row>
     <row r="94" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3522,10 +3419,10 @@
         <v>5</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3551,10 +3448,10 @@
         <v>5</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3580,10 +3477,10 @@
         <v>5</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3609,10 +3506,10 @@
         <v>5</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3638,10 +3535,10 @@
         <v>5</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3667,10 +3564,10 @@
         <v>5</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3696,10 +3593,10 @@
         <v>5</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3725,10 +3622,10 @@
         <v>5</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3754,10 +3651,10 @@
         <v>5</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3783,10 +3680,10 @@
         <v>5</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3812,10 +3709,10 @@
         <v>5</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="I105" s="2" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3841,10 +3738,10 @@
         <v>5</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3870,10 +3767,10 @@
         <v>5</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="I107" s="2" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3899,10 +3796,10 @@
         <v>5</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="I108" s="2" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3928,10 +3825,10 @@
         <v>5</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="I109" s="2" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3957,10 +3854,10 @@
         <v>5</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="I110" s="2" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3986,10 +3883,10 @@
         <v>5</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4015,10 +3912,10 @@
         <v>5</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4044,10 +3941,10 @@
         <v>5</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4073,10 +3970,10 @@
         <v>5</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="I114" s="2" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4100,7 +3997,7 @@
       </c>
       <c r="H115" s="2"/>
       <c r="I115" s="2" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4124,7 +4021,7 @@
       </c>
       <c r="H116" s="2"/>
       <c r="I116" s="2" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4148,7 +4045,7 @@
       </c>
       <c r="H117" s="2"/>
       <c r="I117" s="2" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4172,7 +4069,7 @@
       </c>
       <c r="H118" s="2"/>
       <c r="I118" s="2" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4196,12 +4093,12 @@
       </c>
       <c r="H119" s="2"/>
       <c r="I119" s="2" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="120" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="15" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -4227,10 +4124,10 @@
         <v>5</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -4256,10 +4153,10 @@
         <v>5</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -4285,10 +4182,10 @@
         <v>5</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -4314,10 +4211,10 @@
         <v>5</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -4343,10 +4240,10 @@
         <v>5</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -4372,10 +4269,10 @@
         <v>5</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -4401,10 +4298,10 @@
         <v>5</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -4430,10 +4327,10 @@
         <v>5</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>